<commit_message>
Add 4 more cases for Expedia CarsPage
</commit_message>
<xml_diff>
--- a/com.expedia/src/test/resources/ExpediaData.xlsx
+++ b/com.expedia/src/test/resources/ExpediaData.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafiz\IDEA Project\Team1BootCamp\base\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdaziz/IdeaProjects/Team1BootCamp/com.expedia/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4722EE68-90EB-42C0-AF92-D8B589C2F532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0609926-2B9B-F545-8F9C-B05799977287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
-    <sheet name="Expedia" sheetId="1" r:id="rId1"/>
+    <sheet name="ExpediaAppData" sheetId="1" r:id="rId1"/>
     <sheet name="Ebay" sheetId="2" r:id="rId2"/>
     <sheet name="CBSSports" sheetId="3" r:id="rId3"/>
     <sheet name="ATT" sheetId="4" r:id="rId4"/>
@@ -47,22 +47,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>USA +1</t>
+  </si>
+  <si>
+    <t>Turkey +90</t>
+  </si>
+  <si>
+    <t>Bangladesh +880</t>
+  </si>
+  <si>
+    <t>8454730401</t>
+  </si>
+  <si>
+    <t>1915188515</t>
+  </si>
+  <si>
+    <t>3874837488</t>
+  </si>
+  <si>
+    <t>1234</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,8 +118,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,12 +436,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F16D271-5906-41EE-853E-85EA245B6942}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -419,7 +501,7 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -433,7 +515,7 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -447,7 +529,7 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -461,7 +543,7 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -475,7 +557,7 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -489,7 +571,7 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -503,7 +585,7 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -517,7 +599,7 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -531,9 +613,9 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +633,7 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -563,7 +645,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -575,7 +657,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -587,7 +669,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 9 test cases for CBSSprots SoccerPage
</commit_message>
<xml_diff>
--- a/com.expedia/src/test/resources/ExpediaData.xlsx
+++ b/com.expedia/src/test/resources/ExpediaData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdaziz/IdeaProjects/Team1BootCamp/com.expedia/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0609926-2B9B-F545-8F9C-B05799977287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B35749C-01DF-924C-8526-62FC33A63470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="12860" windowHeight="10420" activeTab="1" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="ExpediaAppData" sheetId="1" r:id="rId1"/>
-    <sheet name="Ebay" sheetId="2" r:id="rId2"/>
+    <sheet name="ExpediaTestData" sheetId="2" r:id="rId2"/>
     <sheet name="CBSSports" sheetId="3" r:id="rId3"/>
     <sheet name="ATT" sheetId="4" r:id="rId4"/>
     <sheet name="BankOfAmerica" sheetId="5" r:id="rId5"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>A</t>
   </si>
@@ -77,6 +77,63 @@
   </si>
   <si>
     <t>1234</t>
+  </si>
+  <si>
+    <t>PickUp</t>
+  </si>
+  <si>
+    <t>DropOff</t>
+  </si>
+  <si>
+    <t>LGA</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>PickUpDay</t>
+  </si>
+  <si>
+    <t>Newark</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>PickMonth</t>
+  </si>
+  <si>
+    <t>PickYear</t>
+  </si>
+  <si>
+    <t>DropDay</t>
+  </si>
+  <si>
+    <t>DropMonth</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -438,7 +495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F16D271-5906-41EE-853E-85EA245B6942}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -565,14 +622,89 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9751B09C-FE73-4F13-A91B-81E55B55AAEA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add 3 more test cases for Expedia CarsPage
</commit_message>
<xml_diff>
--- a/com.expedia/src/test/resources/ExpediaData.xlsx
+++ b/com.expedia/src/test/resources/ExpediaData.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdaziz/IdeaProjects/Team1BootCamp/com.expedia/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B35749C-01DF-924C-8526-62FC33A63470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA022E0E-618D-6246-9178-E65800F8D4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="12860" windowHeight="10420" activeTab="1" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21120" windowHeight="14900" activeTab="1" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="ExpediaAppData" sheetId="1" r:id="rId1"/>
     <sheet name="ExpediaTestData" sheetId="2" r:id="rId2"/>
-    <sheet name="CBSSports" sheetId="3" r:id="rId3"/>
+    <sheet name="Time" sheetId="3" r:id="rId3"/>
     <sheet name="ATT" sheetId="4" r:id="rId4"/>
     <sheet name="BankOfAmerica" sheetId="5" r:id="rId5"/>
     <sheet name="BMWUSA" sheetId="6" r:id="rId6"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>A</t>
   </si>
@@ -134,6 +134,21 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>12:00 AM</t>
+  </si>
+  <si>
+    <t>12:15 AM</t>
+  </si>
+  <si>
+    <t>8:30 am</t>
+  </si>
+  <si>
+    <t>6:30 pm</t>
   </si>
 </sst>
 </file>
@@ -175,10 +190,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,10 +640,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9751B09C-FE73-4F13-A91B-81E55B55AAEA}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -635,7 +653,7 @@
     <col min="7" max="7" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -657,8 +675,11 @@
       <c r="G1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -680,8 +701,11 @@
       <c r="G2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -702,6 +726,9 @@
       </c>
       <c r="G3" t="s">
         <v>21</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -711,14 +738,500 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A517B4-AB0A-4E50-8324-F3955FA294DA}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>2.0833333333333301E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>4.1666666666666699E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>5.2083333333333301E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>7.2916666666666699E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>8.3333333333333301E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>0.104166666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>0.114583333333333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>0.13541666666666699</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>0.14583333333333301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>0.15625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>0.16666666666666699</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>0.17708333333333301</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>0.19791666666666699</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>0.20833333333333301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>0.21875</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>0.22916666666666699</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>0.23958333333333301</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>0.26041666666666702</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>0.27083333333333298</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>0.28125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>0.29166666666666702</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>0.30208333333333298</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>0.32291666666666702</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>0.34375</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
+        <v>0.35416666666666702</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>0.36458333333333298</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>0.38541666666666702</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>0.39583333333333298</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>0.40625</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
+        <v>0.41666666666666702</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
+        <v>0.42708333333333298</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
+        <v>0.44791666666666702</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>0.45833333333333298</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>0.46875</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>0.47916666666666702</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="3">
+        <v>0.48958333333333298</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
+        <v>0.51041666666666696</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
+        <v>0.52083333333333304</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>0.53125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="3">
+        <v>0.54166666666666696</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="3">
+        <v>0.55208333333333304</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="3">
+        <v>0.57291666666666696</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="3">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="3">
+        <v>0.59375</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="3">
+        <v>0.60416666666666696</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="3">
+        <v>0.61458333333333304</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="3">
+        <v>0.63541666666666696</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="3">
+        <v>0.64583333333333304</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="3">
+        <v>0.65625</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="3">
+        <v>0.66666666666666696</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="3">
+        <v>0.67708333333333304</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="3">
+        <v>0.6875</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="3">
+        <v>0.69791666666666696</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="3">
+        <v>0.70833333333333304</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="3">
+        <v>0.71875</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="3">
+        <v>0.72916666666666696</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="3">
+        <v>0.73958333333333304</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="3">
+        <v>0.76041666666666696</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="3">
+        <v>0.77083333333333304</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="3">
+        <v>0.78125</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="3">
+        <v>0.79166666666666696</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="3">
+        <v>0.80208333333333304</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="3">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="3">
+        <v>0.82291666666666696</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="3">
+        <v>0.83333333333333304</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="3">
+        <v>0.84375</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="3">
+        <v>0.85416666666666696</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="3">
+        <v>0.86458333333333304</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="3">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="3">
+        <v>0.88541666666666696</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="3">
+        <v>0.89583333333333304</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="3">
+        <v>0.90625</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="3">
+        <v>0.91666666666666696</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="3">
+        <v>0.92708333333333304</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" s="3">
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="3">
+        <v>0.94791666666666696</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="3">
+        <v>0.95833333333333304</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="3">
+        <v>0.96875</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" s="3">
+        <v>0.97916666666666696</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="3">
+        <v>0.98958333333333304</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>